<commit_message>
sua chi tiet, xuat mat
</commit_message>
<xml_diff>
--- a/DowloadBaoMat.xlsx
+++ b/DowloadBaoMat.xlsx
@@ -29,7 +29,7 @@
     <t>---------o0o---------</t>
   </si>
   <si>
-    <t>Ngày: 14/04/2023</t>
+    <t>Ngày: 16/04/2023</t>
   </si>
   <si>
     <t>STT</t>
@@ -179,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -195,14 +195,8 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -524,15 +518,15 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="9" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="true" style="2"/>
-    <col min="2" max="2" width="24.77734375" customWidth="true" style="2"/>
-    <col min="3" max="3" width="20" customWidth="true" style="2"/>
-    <col min="4" max="4" width="32.33203125" customWidth="true" style="2"/>
+    <col min="2" max="2" width="9.6640625" customWidth="true" style="2"/>
+    <col min="3" max="3" width="11.44140625" customWidth="true" style="2"/>
+    <col min="4" max="4" width="11.109375" customWidth="true" style="2"/>
     <col min="5" max="5" width="17.44140625" customWidth="true" style="2"/>
     <col min="6" max="6" width="21.44140625" customWidth="true" style="2"/>
     <col min="7" max="7" width="21.44140625" customWidth="true" style="2"/>
@@ -542,185 +536,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" customHeight="1" ht="18.6">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:10" customHeight="1" ht="18.6">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="10" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:10">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:10" customHeight="1" ht="50.4">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" customHeight="1" ht="50.4">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>10</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>2</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" customHeight="1" ht="50.4">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>10</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>2</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="11"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="8"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>